<commit_message>
fixed some commandlind issued
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -19,15 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>kom218@lehigh.edu</t>
   </si>
   <si>
     <t>komelm13@gmail.com</t>
-  </si>
-  <si>
-    <t>wahida.merchant@att.net</t>
   </si>
 </sst>
 </file>
@@ -407,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -434,14 +431,6 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>40</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>

</xml_diff>